<commit_message>
Eliminate raw data tab. Wasn't working.
</commit_message>
<xml_diff>
--- a/inst/extdata/Testing new_R_ps/new_R_ps_example.xlsx
+++ b/inst/extdata/Testing new_R_ps/new_R_ps_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/Recca/inst/extdata/Testing new_R_ps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E28F15-70C0-CF4F-A172-E1B31A5CB28E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47888087-2F69-5B43-9597-612A6F677A56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Meta" sheetId="10" r:id="rId1"/>
     <sheet name="PSUT" sheetId="8" r:id="rId2"/>
     <sheet name="Rev Upstream swim Rev" sheetId="12" r:id="rId3"/>
-    <sheet name="RawECCData" sheetId="11" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
@@ -710,7 +709,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="120">
   <si>
     <t>Buildings</t>
   </si>
@@ -2187,73 +2186,10 @@
     </r>
   </si>
   <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Ledger.side</t>
-  </si>
-  <si>
-    <t>Flow.aggregation.point</t>
-  </si>
-  <si>
-    <t>Energy.type</t>
-  </si>
-  <si>
-    <t>Last.stage</t>
-  </si>
-  <si>
-    <t>Flow</t>
-  </si>
-  <si>
-    <t>Product</t>
-  </si>
-  <si>
-    <t>Unit</t>
-  </si>
-  <si>
-    <t>Supply</t>
-  </si>
-  <si>
-    <t>Total primary energy supply</t>
-  </si>
-  <si>
     <t>Resources - Rens</t>
   </si>
   <si>
-    <t>ktoe</t>
-  </si>
-  <si>
-    <t>Transformation processes</t>
-  </si>
-  <si>
-    <t>Gm3-K</t>
-  </si>
-  <si>
-    <t>Energy industry own use</t>
-  </si>
-  <si>
-    <t>Consumption</t>
-  </si>
-  <si>
-    <t>Commercial and public services</t>
-  </si>
-  <si>
     <t>Transport</t>
-  </si>
-  <si>
-    <t>Example</t>
-  </si>
-  <si>
-    <t>Services</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>E.dot</t>
   </si>
   <si>
     <t>This workbook investigates use of a direct (reversing) method to determine the effect of a change in resources available to an ECC.</t>
@@ -3487,7 +3423,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3496,20 +3432,20 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -23757,32 +23693,32 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -23798,7 +23734,7 @@
   </sheetPr>
   <dimension ref="A1:CO144"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="J17" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
@@ -23981,11 +23917,11 @@
     </row>
     <row r="26" spans="1:93" x14ac:dyDescent="0.2">
       <c r="B26" s="10"/>
-      <c r="C26" s="66" t="s">
+      <c r="C26" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="66"/>
-      <c r="E26" s="66"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="60"/>
       <c r="F26" s="39"/>
       <c r="G26" s="39"/>
     </row>
@@ -24254,11 +24190,11 @@
       <c r="CO35" s="31"/>
     </row>
     <row r="36" spans="1:93" ht="18" x14ac:dyDescent="0.25">
-      <c r="C36" s="66" t="s">
+      <c r="C36" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="D36" s="66"/>
-      <c r="E36" s="66"/>
+      <c r="D36" s="60"/>
+      <c r="E36" s="60"/>
       <c r="F36" s="39"/>
       <c r="G36" s="39"/>
       <c r="BM36" s="31"/>
@@ -24476,7 +24412,7 @@
       </c>
       <c r="V41" s="28"/>
       <c r="W41" s="2" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="X41" s="2" t="s">
         <v>58</v>
@@ -24584,7 +24520,7 @@
         <v>18</v>
       </c>
       <c r="CJ41" s="2" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="CK41" s="2" t="s">
         <v>58</v>
@@ -26392,14 +26328,14 @@
       <c r="AA53" s="15"/>
     </row>
     <row r="54" spans="1:93" ht="20" x14ac:dyDescent="0.25">
-      <c r="L54" s="64" t="s">
+      <c r="L54" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="M54" s="64"/>
-      <c r="N54" s="64"/>
-      <c r="O54" s="64"/>
-      <c r="P54" s="64"/>
-      <c r="Q54" s="64"/>
+      <c r="M54" s="63"/>
+      <c r="N54" s="63"/>
+      <c r="O54" s="63"/>
+      <c r="P54" s="63"/>
+      <c r="Q54" s="63"/>
     </row>
     <row r="55" spans="1:93" x14ac:dyDescent="0.2">
       <c r="L55" s="6">
@@ -26439,11 +26375,11 @@
     </row>
     <row r="60" spans="1:93" x14ac:dyDescent="0.2">
       <c r="B60" s="1"/>
-      <c r="Z60" s="66" t="s">
+      <c r="Z60" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="AA60" s="66"/>
-      <c r="AB60" s="66"/>
+      <c r="AA60" s="60"/>
+      <c r="AB60" s="60"/>
       <c r="AI60" s="59" t="s">
         <v>3</v>
       </c>
@@ -27579,11 +27515,11 @@
       <c r="J68" s="59"/>
       <c r="X68" s="15"/>
       <c r="Y68" s="15"/>
-      <c r="Z68" s="64" t="s">
+      <c r="Z68" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="AA68" s="64"/>
-      <c r="AB68" s="64"/>
+      <c r="AA68" s="63"/>
+      <c r="AB68" s="63"/>
       <c r="AD68" s="34" t="s">
         <v>71</v>
       </c>
@@ -27789,17 +27725,17 @@
       <c r="W73" s="15"/>
       <c r="X73" s="15"/>
       <c r="Y73" s="15"/>
-      <c r="Z73" s="66" t="s">
+      <c r="Z73" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="AA73" s="66"/>
-      <c r="AI73" s="67" t="s">
+      <c r="AA73" s="60"/>
+      <c r="AI73" s="64" t="s">
         <v>52</v>
       </c>
-      <c r="AJ73" s="67"/>
+      <c r="AJ73" s="64"/>
       <c r="AK73" s="31"/>
-      <c r="AL73" s="67"/>
-      <c r="AM73" s="67"/>
+      <c r="AL73" s="64"/>
+      <c r="AM73" s="64"/>
       <c r="AN73" s="31"/>
       <c r="AO73" s="31"/>
       <c r="AP73" s="31"/>
@@ -28132,29 +28068,29 @@
       <c r="AD77" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="AI77" s="63" t="s">
+      <c r="AI77" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="AJ77" s="63"/>
+      <c r="AJ77" s="66"/>
       <c r="AK77" s="29"/>
-      <c r="AL77" s="63"/>
-      <c r="AM77" s="63"/>
+      <c r="AL77" s="66"/>
+      <c r="AM77" s="66"/>
       <c r="AN77" s="29"/>
       <c r="AO77" s="31"/>
       <c r="AP77" s="31"/>
       <c r="AQ77" s="31"/>
       <c r="AR77" s="31"/>
       <c r="AS77" s="31"/>
-      <c r="AT77" s="63" t="s">
+      <c r="AT77" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="AU77" s="63"/>
-      <c r="AV77" s="63"/>
-      <c r="AW77" s="63"/>
-      <c r="AX77" s="63"/>
-      <c r="AY77" s="63"/>
-      <c r="AZ77" s="63"/>
-      <c r="BA77" s="63"/>
+      <c r="AU77" s="66"/>
+      <c r="AV77" s="66"/>
+      <c r="AW77" s="66"/>
+      <c r="AX77" s="66"/>
+      <c r="AY77" s="66"/>
+      <c r="AZ77" s="66"/>
+      <c r="BA77" s="66"/>
     </row>
     <row r="78" spans="1:78" x14ac:dyDescent="0.2">
       <c r="B78" s="1"/>
@@ -28254,16 +28190,16 @@
       </c>
     </row>
     <row r="81" spans="1:93" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C81" s="60" t="s">
+      <c r="C81" s="67" t="s">
         <v>85</v>
       </c>
-      <c r="D81" s="60"/>
-      <c r="E81" s="60"/>
-      <c r="F81" s="60"/>
-      <c r="G81" s="60"/>
-      <c r="H81" s="60"/>
-      <c r="I81" s="60"/>
-      <c r="J81" s="60"/>
+      <c r="D81" s="67"/>
+      <c r="E81" s="67"/>
+      <c r="F81" s="67"/>
+      <c r="G81" s="67"/>
+      <c r="H81" s="67"/>
+      <c r="I81" s="67"/>
+      <c r="J81" s="67"/>
       <c r="AI81" s="59" t="s">
         <v>4</v>
       </c>
@@ -29679,14 +29615,14 @@
       </c>
     </row>
     <row r="91" spans="1:93" ht="19" x14ac:dyDescent="0.2">
-      <c r="L91" s="60" t="s">
+      <c r="L91" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="M91" s="60"/>
-      <c r="N91" s="60"/>
-      <c r="O91" s="60"/>
-      <c r="P91" s="60"/>
-      <c r="Q91" s="60"/>
+      <c r="M91" s="67"/>
+      <c r="N91" s="67"/>
+      <c r="O91" s="67"/>
+      <c r="P91" s="67"/>
+      <c r="Q91" s="67"/>
       <c r="Z91" s="41" t="s">
         <v>11</v>
       </c>
@@ -29839,14 +29775,14 @@
       <c r="AA94" s="17"/>
     </row>
     <row r="95" spans="1:93" ht="20" x14ac:dyDescent="0.25">
-      <c r="L95" s="60" t="s">
+      <c r="L95" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="M95" s="60"/>
-      <c r="N95" s="60"/>
-      <c r="O95" s="60"/>
-      <c r="P95" s="60"/>
-      <c r="Q95" s="60"/>
+      <c r="M95" s="67"/>
+      <c r="N95" s="67"/>
+      <c r="O95" s="67"/>
+      <c r="P95" s="67"/>
+      <c r="Q95" s="67"/>
     </row>
     <row r="98" spans="1:40" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="27" t="s">
@@ -30467,16 +30403,16 @@
       </c>
       <c r="D120" s="59"/>
       <c r="E120" s="59"/>
-      <c r="G120" s="60" t="s">
+      <c r="G120" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="H120" s="60"/>
-      <c r="I120" s="60"/>
-      <c r="K120" s="60" t="s">
+      <c r="H120" s="67"/>
+      <c r="I120" s="67"/>
+      <c r="K120" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="L120" s="60"/>
-      <c r="M120" s="60"/>
+      <c r="L120" s="67"/>
+      <c r="M120" s="67"/>
       <c r="N120" s="17"/>
       <c r="O120" s="17" t="s">
         <v>41</v>
@@ -30900,6 +30836,65 @@
     </row>
   </sheetData>
   <mergeCells count="71">
+    <mergeCell ref="A112:I112"/>
+    <mergeCell ref="C143:H143"/>
+    <mergeCell ref="C120:E120"/>
+    <mergeCell ref="G120:I120"/>
+    <mergeCell ref="K120:M120"/>
+    <mergeCell ref="A125:A130"/>
+    <mergeCell ref="C135:H135"/>
+    <mergeCell ref="A137:A142"/>
+    <mergeCell ref="A114:A119"/>
+    <mergeCell ref="BE81:BL81"/>
+    <mergeCell ref="BT81:BY81"/>
+    <mergeCell ref="A83:A90"/>
+    <mergeCell ref="L91:Q91"/>
+    <mergeCell ref="AI91:AP91"/>
+    <mergeCell ref="AT91:BA91"/>
+    <mergeCell ref="BE91:BL91"/>
+    <mergeCell ref="BT91:BY91"/>
+    <mergeCell ref="C81:J81"/>
+    <mergeCell ref="AI81:AP81"/>
+    <mergeCell ref="AT81:BA81"/>
+    <mergeCell ref="J92:J94"/>
+    <mergeCell ref="L95:Q95"/>
+    <mergeCell ref="A100:I100"/>
+    <mergeCell ref="A102:A109"/>
+    <mergeCell ref="C77:J77"/>
+    <mergeCell ref="AI77:AJ77"/>
+    <mergeCell ref="AL77:AM77"/>
+    <mergeCell ref="AT77:BA77"/>
+    <mergeCell ref="C79:J79"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="C68:J68"/>
+    <mergeCell ref="Z68:AB68"/>
+    <mergeCell ref="AI68:AN68"/>
+    <mergeCell ref="AT68:BA68"/>
+    <mergeCell ref="C70:J70"/>
+    <mergeCell ref="Z73:AA73"/>
+    <mergeCell ref="AI73:AJ73"/>
+    <mergeCell ref="AL73:AM73"/>
+    <mergeCell ref="AT73:BA73"/>
+    <mergeCell ref="BE68:BL68"/>
+    <mergeCell ref="BT68:BY68"/>
+    <mergeCell ref="Z60:AB60"/>
+    <mergeCell ref="AI60:AN60"/>
+    <mergeCell ref="AT60:BA60"/>
+    <mergeCell ref="BE60:BL60"/>
+    <mergeCell ref="BT60:BY60"/>
+    <mergeCell ref="A62:A67"/>
+    <mergeCell ref="BE50:BJ50"/>
+    <mergeCell ref="BT50:BY50"/>
+    <mergeCell ref="CA50:CH50"/>
+    <mergeCell ref="J51:J53"/>
+    <mergeCell ref="L54:Q54"/>
+    <mergeCell ref="L56:Q56"/>
+    <mergeCell ref="AT50:AY50"/>
+    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="U42:U49"/>
+    <mergeCell ref="L50:Q50"/>
+    <mergeCell ref="W50:X50"/>
+    <mergeCell ref="AI50:AP50"/>
     <mergeCell ref="CJ40:CK40"/>
     <mergeCell ref="C26:E26"/>
     <mergeCell ref="A28:A35"/>
@@ -30912,65 +30907,6 @@
     <mergeCell ref="BE40:BJ40"/>
     <mergeCell ref="BT40:BY40"/>
     <mergeCell ref="CA40:CH40"/>
-    <mergeCell ref="A42:A49"/>
-    <mergeCell ref="U42:U49"/>
-    <mergeCell ref="L50:Q50"/>
-    <mergeCell ref="W50:X50"/>
-    <mergeCell ref="AI50:AP50"/>
-    <mergeCell ref="A62:A67"/>
-    <mergeCell ref="BE50:BJ50"/>
-    <mergeCell ref="BT50:BY50"/>
-    <mergeCell ref="CA50:CH50"/>
-    <mergeCell ref="J51:J53"/>
-    <mergeCell ref="L54:Q54"/>
-    <mergeCell ref="L56:Q56"/>
-    <mergeCell ref="AT50:AY50"/>
-    <mergeCell ref="BT68:BY68"/>
-    <mergeCell ref="Z60:AB60"/>
-    <mergeCell ref="AI60:AN60"/>
-    <mergeCell ref="AT60:BA60"/>
-    <mergeCell ref="BE60:BL60"/>
-    <mergeCell ref="BT60:BY60"/>
-    <mergeCell ref="Z73:AA73"/>
-    <mergeCell ref="AI73:AJ73"/>
-    <mergeCell ref="AL73:AM73"/>
-    <mergeCell ref="AT73:BA73"/>
-    <mergeCell ref="BE68:BL68"/>
-    <mergeCell ref="C68:J68"/>
-    <mergeCell ref="Z68:AB68"/>
-    <mergeCell ref="AI68:AN68"/>
-    <mergeCell ref="AT68:BA68"/>
-    <mergeCell ref="C70:J70"/>
-    <mergeCell ref="AI77:AJ77"/>
-    <mergeCell ref="AL77:AM77"/>
-    <mergeCell ref="AT77:BA77"/>
-    <mergeCell ref="C79:J79"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="J92:J94"/>
-    <mergeCell ref="L95:Q95"/>
-    <mergeCell ref="A100:I100"/>
-    <mergeCell ref="A102:A109"/>
-    <mergeCell ref="C77:J77"/>
-    <mergeCell ref="BE81:BL81"/>
-    <mergeCell ref="BT81:BY81"/>
-    <mergeCell ref="A83:A90"/>
-    <mergeCell ref="L91:Q91"/>
-    <mergeCell ref="AI91:AP91"/>
-    <mergeCell ref="AT91:BA91"/>
-    <mergeCell ref="BE91:BL91"/>
-    <mergeCell ref="BT91:BY91"/>
-    <mergeCell ref="C81:J81"/>
-    <mergeCell ref="AI81:AP81"/>
-    <mergeCell ref="AT81:BA81"/>
-    <mergeCell ref="A112:I112"/>
-    <mergeCell ref="C143:H143"/>
-    <mergeCell ref="C120:E120"/>
-    <mergeCell ref="G120:I120"/>
-    <mergeCell ref="K120:M120"/>
-    <mergeCell ref="A125:A130"/>
-    <mergeCell ref="C135:H135"/>
-    <mergeCell ref="A137:A142"/>
-    <mergeCell ref="A114:A119"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="17" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -30983,8 +30919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5018262C-ADF6-FA4F-AD02-C6E8C0BF89C2}">
   <dimension ref="A1:GE147"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CU46" sqref="CU46"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CU1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -31011,7 +30947,7 @@
   <sheetData>
     <row r="1" spans="1:187" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="68" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="B1" s="68"/>
       <c r="C1" s="68"/>
@@ -31048,7 +30984,7 @@
       <c r="AH1" s="68"/>
       <c r="AI1" s="68"/>
       <c r="CQ1" s="68" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="CR1" s="68"/>
       <c r="CS1" s="68"/>
@@ -31083,7 +31019,7 @@
       <c r="DV1" s="68"/>
       <c r="DW1" s="68"/>
       <c r="EY1" s="68" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="EZ1" s="68"/>
       <c r="FA1" s="68"/>
@@ -31549,11 +31485,11 @@
     </row>
     <row r="29" spans="1:177" x14ac:dyDescent="0.2">
       <c r="B29" s="10"/>
-      <c r="C29" s="66" t="s">
+      <c r="C29" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="66"/>
-      <c r="E29" s="66"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="60"/>
       <c r="F29" s="52"/>
       <c r="G29" s="52"/>
       <c r="N29" s="50"/>
@@ -31898,11 +31834,11 @@
       <c r="CN38" s="31"/>
     </row>
     <row r="39" spans="1:179" ht="18" x14ac:dyDescent="0.25">
-      <c r="C39" s="66" t="s">
+      <c r="C39" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="D39" s="66"/>
-      <c r="E39" s="66"/>
+      <c r="D39" s="60"/>
+      <c r="E39" s="60"/>
       <c r="F39" s="52"/>
       <c r="G39" s="52"/>
       <c r="BM39" s="31"/>
@@ -32170,7 +32106,7 @@
       </c>
       <c r="V44" s="28"/>
       <c r="W44" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="X44" s="2" t="s">
         <v>21</v>
@@ -32278,7 +32214,7 @@
         <v>18</v>
       </c>
       <c r="CJ44" s="2" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="CK44" s="2" t="s">
         <v>58</v>
@@ -32289,7 +32225,7 @@
       <c r="CO44" s="58"/>
       <c r="CT44" s="28"/>
       <c r="CU44" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="CV44" s="2" t="s">
         <v>21</v>
@@ -32337,7 +32273,7 @@
         <v>16</v>
       </c>
       <c r="EC44" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="ED44" s="2" t="s">
         <v>21</v>
@@ -32386,7 +32322,7 @@
         <v>16</v>
       </c>
       <c r="FT44" s="2" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="FU44" s="2" t="s">
         <v>58</v>
@@ -34819,14 +34755,14 @@
       <c r="CN53" s="8"/>
       <c r="CO53" s="57"/>
       <c r="CU53" s="59" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="CV53" s="59"/>
       <c r="CX53" s="46" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="DV53" s="59" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="DW53" s="59"/>
       <c r="DX53" s="59"/>
@@ -34835,11 +34771,11 @@
       <c r="EA53" s="59"/>
       <c r="EB53" s="8"/>
       <c r="EC53" s="59" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="ED53" s="59"/>
       <c r="EF53" s="46" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="EG53" s="8"/>
       <c r="EH53" s="8"/>
@@ -34859,7 +34795,7 @@
       <c r="EV53" s="8"/>
       <c r="EW53" s="57"/>
       <c r="FM53" s="59" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="FN53" s="59"/>
       <c r="FO53" s="59"/>
@@ -34868,11 +34804,11 @@
       <c r="FR53" s="59"/>
       <c r="FS53" s="8"/>
       <c r="FT53" s="59" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="FU53" s="59"/>
       <c r="FW53" s="46" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="FX53" s="8"/>
     </row>
@@ -34999,14 +34935,14 @@
       <c r="AA56" s="15"/>
     </row>
     <row r="57" spans="1:180" ht="20" x14ac:dyDescent="0.25">
-      <c r="L57" s="64" t="s">
+      <c r="L57" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="M57" s="64"/>
-      <c r="N57" s="64"/>
-      <c r="O57" s="64"/>
-      <c r="P57" s="64"/>
-      <c r="Q57" s="64"/>
+      <c r="M57" s="63"/>
+      <c r="N57" s="63"/>
+      <c r="O57" s="63"/>
+      <c r="P57" s="63"/>
+      <c r="Q57" s="63"/>
     </row>
     <row r="58" spans="1:180" x14ac:dyDescent="0.2">
       <c r="L58" s="6">
@@ -35046,11 +34982,11 @@
     </row>
     <row r="63" spans="1:180" x14ac:dyDescent="0.2">
       <c r="B63" s="1"/>
-      <c r="Z63" s="66" t="s">
+      <c r="Z63" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="AA63" s="66"/>
-      <c r="AB63" s="66"/>
+      <c r="AA63" s="60"/>
+      <c r="AB63" s="60"/>
       <c r="AI63" s="59" t="s">
         <v>3</v>
       </c>
@@ -36793,11 +36729,11 @@
       <c r="J71" s="59"/>
       <c r="X71" s="15"/>
       <c r="Y71" s="15"/>
-      <c r="Z71" s="64" t="s">
+      <c r="Z71" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="AA71" s="64"/>
-      <c r="AB71" s="64"/>
+      <c r="AA71" s="63"/>
+      <c r="AB71" s="63"/>
       <c r="AD71" s="34" t="s">
         <v>71</v>
       </c>
@@ -36853,10 +36789,10 @@
       <c r="BY71" s="62"/>
       <c r="BZ71" s="26"/>
       <c r="CX71" s="46" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="DB71" s="59" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="DC71" s="59"/>
       <c r="DD71" s="59"/>
@@ -36869,7 +36805,7 @@
       <c r="DK71" s="8"/>
       <c r="DL71" s="8"/>
       <c r="DM71" s="59" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="DN71" s="59"/>
       <c r="DO71" s="59"/>
@@ -36892,7 +36828,7 @@
       <c r="FB71" s="8"/>
       <c r="FC71" s="8"/>
       <c r="FD71" s="59" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="FE71" s="59"/>
       <c r="FF71" s="59"/>
@@ -37063,18 +36999,18 @@
       <c r="W76" s="15"/>
       <c r="X76" s="15"/>
       <c r="Y76" s="15"/>
-      <c r="Z76" s="66" t="s">
+      <c r="Z76" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="AA76" s="66"/>
-      <c r="AB76" s="66"/>
-      <c r="AI76" s="67" t="s">
+      <c r="AA76" s="60"/>
+      <c r="AB76" s="60"/>
+      <c r="AI76" s="64" t="s">
         <v>52</v>
       </c>
-      <c r="AJ76" s="67"/>
+      <c r="AJ76" s="64"/>
       <c r="AK76" s="31"/>
-      <c r="AL76" s="67"/>
-      <c r="AM76" s="67"/>
+      <c r="AL76" s="64"/>
+      <c r="AM76" s="64"/>
       <c r="AN76" s="31"/>
       <c r="AO76" s="31"/>
       <c r="AP76" s="31"/>
@@ -37136,7 +37072,7 @@
         <v>33</v>
       </c>
       <c r="AI77" s="2" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="AJ77" s="2" t="s">
         <v>58</v>
@@ -37204,7 +37140,7 @@
         <v>84</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="C78" s="4">
         <v>0</v>
@@ -37345,7 +37281,7 @@
         <v>84</v>
       </c>
       <c r="DL78" s="1" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="DM78" s="6">
         <f t="array" aca="1" ref="DM78:DT79" ca="1">MMULT(BE78:BL79, DB86:DI93)</f>
@@ -37383,7 +37319,7 @@
         <v>84</v>
       </c>
       <c r="FC78" s="47" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="FD78" s="6">
         <f t="array" ref="FD78:FK79">TRANSPOSE(EC45:ED52)</f>
@@ -37647,42 +37583,42 @@
       <c r="AD80" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="AI80" s="63" t="s">
+      <c r="AI80" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="AJ80" s="63"/>
+      <c r="AJ80" s="66"/>
       <c r="AK80" s="29"/>
-      <c r="AL80" s="63"/>
-      <c r="AM80" s="63"/>
+      <c r="AL80" s="66"/>
+      <c r="AM80" s="66"/>
       <c r="AN80" s="29"/>
       <c r="AO80" s="31"/>
       <c r="AP80" s="31"/>
       <c r="AQ80" s="31"/>
       <c r="AR80" s="31"/>
       <c r="AS80" s="31"/>
-      <c r="AT80" s="63" t="s">
+      <c r="AT80" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="AU80" s="63"/>
-      <c r="AV80" s="63"/>
-      <c r="AW80" s="63"/>
-      <c r="AX80" s="63"/>
-      <c r="AY80" s="63"/>
-      <c r="AZ80" s="63"/>
-      <c r="BA80" s="63"/>
-      <c r="BE80" s="63" t="s">
-        <v>126</v>
-      </c>
-      <c r="BF80" s="63"/>
-      <c r="BG80" s="63"/>
-      <c r="BH80" s="63"/>
-      <c r="BI80" s="63"/>
-      <c r="BJ80" s="63"/>
-      <c r="BK80" s="63"/>
-      <c r="BL80" s="63"/>
+      <c r="AU80" s="66"/>
+      <c r="AV80" s="66"/>
+      <c r="AW80" s="66"/>
+      <c r="AX80" s="66"/>
+      <c r="AY80" s="66"/>
+      <c r="AZ80" s="66"/>
+      <c r="BA80" s="66"/>
+      <c r="BE80" s="66" t="s">
+        <v>105</v>
+      </c>
+      <c r="BF80" s="66"/>
+      <c r="BG80" s="66"/>
+      <c r="BH80" s="66"/>
+      <c r="BI80" s="66"/>
+      <c r="BJ80" s="66"/>
+      <c r="BK80" s="66"/>
+      <c r="BL80" s="66"/>
       <c r="DL80" s="1"/>
       <c r="DM80" s="59" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="DN80" s="59"/>
       <c r="DO80" s="59"/>
@@ -37693,7 +37629,7 @@
       <c r="DT80" s="59"/>
       <c r="FC80" s="1"/>
       <c r="FD80" s="59" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="FE80" s="59"/>
       <c r="FF80" s="59"/>
@@ -37801,16 +37737,16 @@
       </c>
     </row>
     <row r="84" spans="1:174" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C84" s="60" t="s">
+      <c r="C84" s="67" t="s">
         <v>85</v>
       </c>
-      <c r="D84" s="60"/>
-      <c r="E84" s="60"/>
-      <c r="F84" s="60"/>
-      <c r="G84" s="60"/>
-      <c r="H84" s="60"/>
-      <c r="I84" s="60"/>
-      <c r="J84" s="60"/>
+      <c r="D84" s="67"/>
+      <c r="E84" s="67"/>
+      <c r="F84" s="67"/>
+      <c r="G84" s="67"/>
+      <c r="H84" s="67"/>
+      <c r="I84" s="67"/>
+      <c r="J84" s="67"/>
       <c r="AI84" s="59" t="s">
         <v>4</v>
       </c>
@@ -40018,14 +39954,14 @@
       </c>
     </row>
     <row r="94" spans="1:174" ht="19" x14ac:dyDescent="0.2">
-      <c r="L94" s="60" t="s">
+      <c r="L94" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="M94" s="60"/>
-      <c r="N94" s="60"/>
-      <c r="O94" s="60"/>
-      <c r="P94" s="60"/>
-      <c r="Q94" s="60"/>
+      <c r="M94" s="67"/>
+      <c r="N94" s="67"/>
+      <c r="O94" s="67"/>
+      <c r="P94" s="67"/>
+      <c r="Q94" s="67"/>
       <c r="Z94" s="46" t="s">
         <v>11</v>
       </c>
@@ -40092,10 +40028,10 @@
       <c r="CN94" s="8"/>
       <c r="CO94" s="57"/>
       <c r="CX94" s="46" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="DB94" s="59" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="DC94" s="59"/>
       <c r="DD94" s="59"/>
@@ -40105,23 +40041,23 @@
       <c r="DH94" s="59"/>
       <c r="DI94" s="59"/>
       <c r="DJ94" s="8"/>
-      <c r="DV94" s="60" t="s">
-        <v>137</v>
-      </c>
-      <c r="DW94" s="60"/>
-      <c r="DX94" s="60"/>
-      <c r="DY94" s="60"/>
-      <c r="DZ94" s="60"/>
-      <c r="EA94" s="60"/>
+      <c r="DV94" s="67" t="s">
+        <v>116</v>
+      </c>
+      <c r="DW94" s="67"/>
+      <c r="DX94" s="67"/>
+      <c r="DY94" s="67"/>
+      <c r="DZ94" s="67"/>
+      <c r="EA94" s="67"/>
       <c r="EW94" s="57"/>
-      <c r="FM94" s="60" t="s">
-        <v>135</v>
-      </c>
-      <c r="FN94" s="60"/>
-      <c r="FO94" s="60"/>
-      <c r="FP94" s="60"/>
-      <c r="FQ94" s="60"/>
-      <c r="FR94" s="60"/>
+      <c r="FM94" s="67" t="s">
+        <v>114</v>
+      </c>
+      <c r="FN94" s="67"/>
+      <c r="FO94" s="67"/>
+      <c r="FP94" s="67"/>
+      <c r="FQ94" s="67"/>
+      <c r="FR94" s="67"/>
     </row>
     <row r="95" spans="1:174" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J95" s="61" t="s">
@@ -40381,30 +40317,30 @@
       </c>
     </row>
     <row r="98" spans="1:174" ht="20" x14ac:dyDescent="0.25">
-      <c r="L98" s="60" t="s">
+      <c r="L98" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="M98" s="60"/>
-      <c r="N98" s="60"/>
-      <c r="O98" s="60"/>
-      <c r="P98" s="60"/>
-      <c r="Q98" s="60"/>
-      <c r="DV98" s="60" t="s">
-        <v>138</v>
-      </c>
-      <c r="DW98" s="60"/>
-      <c r="DX98" s="60"/>
-      <c r="DY98" s="60"/>
-      <c r="DZ98" s="60"/>
-      <c r="EA98" s="60"/>
-      <c r="FM98" s="60" t="s">
-        <v>136</v>
-      </c>
-      <c r="FN98" s="60"/>
-      <c r="FO98" s="60"/>
-      <c r="FP98" s="60"/>
-      <c r="FQ98" s="60"/>
-      <c r="FR98" s="60"/>
+      <c r="M98" s="67"/>
+      <c r="N98" s="67"/>
+      <c r="O98" s="67"/>
+      <c r="P98" s="67"/>
+      <c r="Q98" s="67"/>
+      <c r="DV98" s="67" t="s">
+        <v>117</v>
+      </c>
+      <c r="DW98" s="67"/>
+      <c r="DX98" s="67"/>
+      <c r="DY98" s="67"/>
+      <c r="DZ98" s="67"/>
+      <c r="EA98" s="67"/>
+      <c r="FM98" s="67" t="s">
+        <v>115</v>
+      </c>
+      <c r="FN98" s="67"/>
+      <c r="FO98" s="67"/>
+      <c r="FP98" s="67"/>
+      <c r="FQ98" s="67"/>
+      <c r="FR98" s="67"/>
     </row>
     <row r="101" spans="1:174" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="27" t="s">
@@ -41025,16 +40961,16 @@
       </c>
       <c r="D123" s="59"/>
       <c r="E123" s="59"/>
-      <c r="G123" s="60" t="s">
+      <c r="G123" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="H123" s="60"/>
-      <c r="I123" s="60"/>
-      <c r="K123" s="60" t="s">
+      <c r="H123" s="67"/>
+      <c r="I123" s="67"/>
+      <c r="K123" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="L123" s="60"/>
-      <c r="M123" s="60"/>
+      <c r="L123" s="67"/>
+      <c r="M123" s="67"/>
       <c r="N123" s="17"/>
       <c r="O123" s="17" t="s">
         <v>41</v>
@@ -41458,54 +41394,44 @@
     </row>
   </sheetData>
   <mergeCells count="111">
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="A31:A38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C43:J43"/>
-    <mergeCell ref="L43:Q43"/>
-    <mergeCell ref="W43:X43"/>
-    <mergeCell ref="A45:A52"/>
-    <mergeCell ref="U45:U52"/>
-    <mergeCell ref="L53:Q53"/>
-    <mergeCell ref="W53:X53"/>
-    <mergeCell ref="AI53:AP53"/>
-    <mergeCell ref="AT53:AY53"/>
-    <mergeCell ref="AI43:AP43"/>
-    <mergeCell ref="AT43:AY43"/>
-    <mergeCell ref="BE43:BJ43"/>
-    <mergeCell ref="Z63:AB63"/>
-    <mergeCell ref="AI63:AN63"/>
-    <mergeCell ref="AT63:BA63"/>
-    <mergeCell ref="BE63:BL63"/>
-    <mergeCell ref="BT63:BY63"/>
-    <mergeCell ref="A65:A70"/>
-    <mergeCell ref="BE53:BJ53"/>
-    <mergeCell ref="BT53:BY53"/>
-    <mergeCell ref="CA53:CH53"/>
-    <mergeCell ref="J54:J56"/>
-    <mergeCell ref="L57:Q57"/>
-    <mergeCell ref="L59:Q59"/>
-    <mergeCell ref="C73:J73"/>
-    <mergeCell ref="AI76:AJ76"/>
-    <mergeCell ref="AL76:AM76"/>
-    <mergeCell ref="AT76:BA76"/>
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="C71:J71"/>
-    <mergeCell ref="Z71:AB71"/>
-    <mergeCell ref="AI71:AN71"/>
-    <mergeCell ref="AT71:BA71"/>
-    <mergeCell ref="AI94:AP94"/>
-    <mergeCell ref="AT94:BA94"/>
-    <mergeCell ref="BE94:BL94"/>
-    <mergeCell ref="BT94:BY94"/>
-    <mergeCell ref="C80:J80"/>
-    <mergeCell ref="AI80:AJ80"/>
-    <mergeCell ref="AL80:AM80"/>
-    <mergeCell ref="AT80:BA80"/>
-    <mergeCell ref="C82:J82"/>
-    <mergeCell ref="C84:J84"/>
-    <mergeCell ref="AI84:AP84"/>
-    <mergeCell ref="AT84:BA84"/>
+    <mergeCell ref="FK95:FK97"/>
+    <mergeCell ref="FM98:FR98"/>
+    <mergeCell ref="FM84:FR84"/>
+    <mergeCell ref="DV84:EA84"/>
+    <mergeCell ref="DK86:DK93"/>
+    <mergeCell ref="DV94:EA94"/>
+    <mergeCell ref="DT95:DT97"/>
+    <mergeCell ref="DV98:EA98"/>
+    <mergeCell ref="FB65:FB70"/>
+    <mergeCell ref="FD71:FK71"/>
+    <mergeCell ref="FB78:FB79"/>
+    <mergeCell ref="FD80:FK80"/>
+    <mergeCell ref="FB86:FB93"/>
+    <mergeCell ref="FM94:FR94"/>
+    <mergeCell ref="DK78:DK79"/>
+    <mergeCell ref="DM80:DT80"/>
+    <mergeCell ref="EY1:GE1"/>
+    <mergeCell ref="FD43:FK43"/>
+    <mergeCell ref="FM43:FR43"/>
+    <mergeCell ref="FT43:FU43"/>
+    <mergeCell ref="FB45:FB52"/>
+    <mergeCell ref="FM53:FR53"/>
+    <mergeCell ref="FT53:FU53"/>
+    <mergeCell ref="EC43:ED43"/>
+    <mergeCell ref="EC53:ED53"/>
+    <mergeCell ref="BE76:BL76"/>
+    <mergeCell ref="DB94:DI94"/>
+    <mergeCell ref="DM71:DT71"/>
+    <mergeCell ref="DV53:EA53"/>
+    <mergeCell ref="DV43:EA43"/>
+    <mergeCell ref="DK45:DK52"/>
+    <mergeCell ref="DK65:DK70"/>
+    <mergeCell ref="DM43:DT43"/>
+    <mergeCell ref="BE71:BL71"/>
+    <mergeCell ref="BT71:BY71"/>
+    <mergeCell ref="BT43:BY43"/>
+    <mergeCell ref="CA43:CH43"/>
+    <mergeCell ref="CJ43:CK43"/>
     <mergeCell ref="C146:H146"/>
     <mergeCell ref="Z76:AB76"/>
     <mergeCell ref="A1:AI1"/>
@@ -41530,760 +41456,59 @@
     <mergeCell ref="BT84:BY84"/>
     <mergeCell ref="A86:A93"/>
     <mergeCell ref="L94:Q94"/>
+    <mergeCell ref="BE94:BL94"/>
+    <mergeCell ref="BT94:BY94"/>
+    <mergeCell ref="C80:J80"/>
+    <mergeCell ref="AI80:AJ80"/>
+    <mergeCell ref="AL80:AM80"/>
+    <mergeCell ref="AT80:BA80"/>
+    <mergeCell ref="C82:J82"/>
+    <mergeCell ref="C84:J84"/>
+    <mergeCell ref="AI84:AP84"/>
+    <mergeCell ref="AT84:BA84"/>
     <mergeCell ref="BE80:BL80"/>
-    <mergeCell ref="BE76:BL76"/>
-    <mergeCell ref="DB94:DI94"/>
-    <mergeCell ref="DM71:DT71"/>
-    <mergeCell ref="DV53:EA53"/>
-    <mergeCell ref="DV43:EA43"/>
-    <mergeCell ref="DK45:DK52"/>
-    <mergeCell ref="DK65:DK70"/>
-    <mergeCell ref="DM43:DT43"/>
-    <mergeCell ref="BE71:BL71"/>
-    <mergeCell ref="BT71:BY71"/>
-    <mergeCell ref="BT43:BY43"/>
-    <mergeCell ref="CA43:CH43"/>
-    <mergeCell ref="CJ43:CK43"/>
-    <mergeCell ref="EY1:GE1"/>
-    <mergeCell ref="FD43:FK43"/>
-    <mergeCell ref="FM43:FR43"/>
-    <mergeCell ref="FT43:FU43"/>
-    <mergeCell ref="FB45:FB52"/>
-    <mergeCell ref="FM53:FR53"/>
-    <mergeCell ref="FT53:FU53"/>
-    <mergeCell ref="EC43:ED43"/>
-    <mergeCell ref="EC53:ED53"/>
-    <mergeCell ref="FK95:FK97"/>
-    <mergeCell ref="FM98:FR98"/>
-    <mergeCell ref="FM84:FR84"/>
-    <mergeCell ref="DV84:EA84"/>
-    <mergeCell ref="DK86:DK93"/>
-    <mergeCell ref="DV94:EA94"/>
-    <mergeCell ref="DT95:DT97"/>
-    <mergeCell ref="DV98:EA98"/>
-    <mergeCell ref="FB65:FB70"/>
-    <mergeCell ref="FD71:FK71"/>
-    <mergeCell ref="FB78:FB79"/>
-    <mergeCell ref="FD80:FK80"/>
-    <mergeCell ref="FB86:FB93"/>
-    <mergeCell ref="FM94:FR94"/>
-    <mergeCell ref="DK78:DK79"/>
-    <mergeCell ref="DM80:DT80"/>
+    <mergeCell ref="AI76:AJ76"/>
+    <mergeCell ref="AL76:AM76"/>
+    <mergeCell ref="AT76:BA76"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="C71:J71"/>
+    <mergeCell ref="Z71:AB71"/>
+    <mergeCell ref="AI71:AN71"/>
+    <mergeCell ref="AT71:BA71"/>
+    <mergeCell ref="AI94:AP94"/>
+    <mergeCell ref="AT94:BA94"/>
+    <mergeCell ref="BT63:BY63"/>
+    <mergeCell ref="A65:A70"/>
+    <mergeCell ref="BE53:BJ53"/>
+    <mergeCell ref="BT53:BY53"/>
+    <mergeCell ref="CA53:CH53"/>
+    <mergeCell ref="J54:J56"/>
+    <mergeCell ref="L57:Q57"/>
+    <mergeCell ref="L59:Q59"/>
+    <mergeCell ref="C73:J73"/>
+    <mergeCell ref="AI53:AP53"/>
+    <mergeCell ref="AT53:AY53"/>
+    <mergeCell ref="AI43:AP43"/>
+    <mergeCell ref="AT43:AY43"/>
+    <mergeCell ref="BE43:BJ43"/>
+    <mergeCell ref="Z63:AB63"/>
+    <mergeCell ref="AI63:AN63"/>
+    <mergeCell ref="AT63:BA63"/>
+    <mergeCell ref="BE63:BL63"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="A31:A38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C43:J43"/>
+    <mergeCell ref="L43:Q43"/>
+    <mergeCell ref="W43:X43"/>
+    <mergeCell ref="A45:A52"/>
+    <mergeCell ref="U45:U52"/>
+    <mergeCell ref="L53:Q53"/>
+    <mergeCell ref="W53:X53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81DB1CE6-E3EC-7B4E-8832-2A8872C682BA}">
-  <dimension ref="A1:J21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="7" max="7" width="16.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G1" t="s">
-        <v>97</v>
-      </c>
-      <c r="H1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B2">
-        <v>2000</v>
-      </c>
-      <c r="C2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B3">
-        <v>2000</v>
-      </c>
-      <c r="C3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E3" t="s">
-        <v>112</v>
-      </c>
-      <c r="F3" t="s">
-        <v>111</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B4">
-        <v>2000</v>
-      </c>
-      <c r="C4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E4" t="s">
-        <v>112</v>
-      </c>
-      <c r="F4" t="s">
-        <v>111</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4">
-        <f>-PSUT!L42</f>
-        <v>-97</v>
-      </c>
-      <c r="J4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B5">
-        <v>2000</v>
-      </c>
-      <c r="C5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" t="s">
-        <v>106</v>
-      </c>
-      <c r="E5" t="s">
-        <v>112</v>
-      </c>
-      <c r="F5" t="s">
-        <v>111</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" t="e">
-        <f>-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B6">
-        <v>2000</v>
-      </c>
-      <c r="C6" t="s">
-        <v>100</v>
-      </c>
-      <c r="D6" t="s">
-        <v>104</v>
-      </c>
-      <c r="E6" t="s">
-        <v>112</v>
-      </c>
-      <c r="F6" t="s">
-        <v>111</v>
-      </c>
-      <c r="G6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>110</v>
-      </c>
-      <c r="B7">
-        <v>2000</v>
-      </c>
-      <c r="C7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" t="s">
-        <v>104</v>
-      </c>
-      <c r="E7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F7" t="s">
-        <v>111</v>
-      </c>
-      <c r="G7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" t="e">
-        <f>-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>110</v>
-      </c>
-      <c r="B8">
-        <v>2000</v>
-      </c>
-      <c r="C8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D8" t="s">
-        <v>104</v>
-      </c>
-      <c r="E8" t="s">
-        <v>112</v>
-      </c>
-      <c r="F8" t="s">
-        <v>111</v>
-      </c>
-      <c r="G8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>110</v>
-      </c>
-      <c r="B9">
-        <v>2000</v>
-      </c>
-      <c r="C9" t="s">
-        <v>100</v>
-      </c>
-      <c r="D9" t="s">
-        <v>104</v>
-      </c>
-      <c r="E9" t="s">
-        <v>112</v>
-      </c>
-      <c r="F9" t="s">
-        <v>111</v>
-      </c>
-      <c r="G9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" t="e">
-        <f>-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>110</v>
-      </c>
-      <c r="B10">
-        <v>2000</v>
-      </c>
-      <c r="C10" t="s">
-        <v>100</v>
-      </c>
-      <c r="D10" t="s">
-        <v>104</v>
-      </c>
-      <c r="E10" t="s">
-        <v>112</v>
-      </c>
-      <c r="F10" t="s">
-        <v>111</v>
-      </c>
-      <c r="G10" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" t="s">
-        <v>29</v>
-      </c>
-      <c r="I10" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>110</v>
-      </c>
-      <c r="B11">
-        <v>2000</v>
-      </c>
-      <c r="C11" t="s">
-        <v>100</v>
-      </c>
-      <c r="D11" t="s">
-        <v>104</v>
-      </c>
-      <c r="E11" t="s">
-        <v>112</v>
-      </c>
-      <c r="F11" t="s">
-        <v>111</v>
-      </c>
-      <c r="G11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" t="e">
-        <f>-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>110</v>
-      </c>
-      <c r="B12">
-        <v>2000</v>
-      </c>
-      <c r="C12" t="s">
-        <v>100</v>
-      </c>
-      <c r="D12" t="s">
-        <v>104</v>
-      </c>
-      <c r="E12" t="s">
-        <v>112</v>
-      </c>
-      <c r="F12" t="s">
-        <v>111</v>
-      </c>
-      <c r="G12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>110</v>
-      </c>
-      <c r="B13">
-        <v>2000</v>
-      </c>
-      <c r="C13" t="s">
-        <v>100</v>
-      </c>
-      <c r="D13" t="s">
-        <v>104</v>
-      </c>
-      <c r="E13" t="s">
-        <v>112</v>
-      </c>
-      <c r="F13" t="s">
-        <v>111</v>
-      </c>
-      <c r="G13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I13" t="e">
-        <f>-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J13" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>110</v>
-      </c>
-      <c r="B14">
-        <v>2000</v>
-      </c>
-      <c r="C14" t="s">
-        <v>100</v>
-      </c>
-      <c r="D14" t="s">
-        <v>104</v>
-      </c>
-      <c r="E14" t="s">
-        <v>112</v>
-      </c>
-      <c r="F14" t="s">
-        <v>111</v>
-      </c>
-      <c r="G14" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I14" t="e">
-        <f>-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>110</v>
-      </c>
-      <c r="B15">
-        <v>2000</v>
-      </c>
-      <c r="C15" t="s">
-        <v>100</v>
-      </c>
-      <c r="D15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E15" t="s">
-        <v>112</v>
-      </c>
-      <c r="F15" t="s">
-        <v>111</v>
-      </c>
-      <c r="G15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>110</v>
-      </c>
-      <c r="B16">
-        <v>2000</v>
-      </c>
-      <c r="C16" t="s">
-        <v>100</v>
-      </c>
-      <c r="D16" t="s">
-        <v>104</v>
-      </c>
-      <c r="E16" t="s">
-        <v>112</v>
-      </c>
-      <c r="F16" t="s">
-        <v>111</v>
-      </c>
-      <c r="G16" t="s">
-        <v>0</v>
-      </c>
-      <c r="H16" t="s">
-        <v>29</v>
-      </c>
-      <c r="I16" t="e">
-        <f>-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>110</v>
-      </c>
-      <c r="B17">
-        <v>2000</v>
-      </c>
-      <c r="C17" t="s">
-        <v>100</v>
-      </c>
-      <c r="D17" t="s">
-        <v>104</v>
-      </c>
-      <c r="E17" t="s">
-        <v>112</v>
-      </c>
-      <c r="F17" t="s">
-        <v>111</v>
-      </c>
-      <c r="G17" t="s">
-        <v>0</v>
-      </c>
-      <c r="H17" t="s">
-        <v>26</v>
-      </c>
-      <c r="I17" t="e">
-        <f>-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J17" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>110</v>
-      </c>
-      <c r="B18">
-        <v>2000</v>
-      </c>
-      <c r="C18" t="s">
-        <v>100</v>
-      </c>
-      <c r="D18" t="s">
-        <v>104</v>
-      </c>
-      <c r="E18" t="s">
-        <v>112</v>
-      </c>
-      <c r="F18" t="s">
-        <v>111</v>
-      </c>
-      <c r="G18" t="s">
-        <v>0</v>
-      </c>
-      <c r="H18" t="s">
-        <v>19</v>
-      </c>
-      <c r="I18" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>110</v>
-      </c>
-      <c r="B19">
-        <v>2000</v>
-      </c>
-      <c r="C19" t="s">
-        <v>107</v>
-      </c>
-      <c r="D19" t="s">
-        <v>109</v>
-      </c>
-      <c r="E19" t="s">
-        <v>112</v>
-      </c>
-      <c r="F19" t="s">
-        <v>111</v>
-      </c>
-      <c r="G19" t="s">
-        <v>109</v>
-      </c>
-      <c r="H19" t="s">
-        <v>18</v>
-      </c>
-      <c r="I19" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>110</v>
-      </c>
-      <c r="B20">
-        <v>2000</v>
-      </c>
-      <c r="C20" t="s">
-        <v>107</v>
-      </c>
-      <c r="D20" t="s">
-        <v>109</v>
-      </c>
-      <c r="E20" t="s">
-        <v>112</v>
-      </c>
-      <c r="F20" t="s">
-        <v>111</v>
-      </c>
-      <c r="G20" t="s">
-        <v>109</v>
-      </c>
-      <c r="H20" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>110</v>
-      </c>
-      <c r="B21">
-        <v>2000</v>
-      </c>
-      <c r="C21" t="s">
-        <v>107</v>
-      </c>
-      <c r="D21" t="s">
-        <v>108</v>
-      </c>
-      <c r="E21" t="s">
-        <v>112</v>
-      </c>
-      <c r="F21" t="s">
-        <v>111</v>
-      </c>
-      <c r="G21" t="s">
-        <v>108</v>
-      </c>
-      <c r="H21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I21" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J21" t="s">
-        <v>105</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Working on DS swim
</commit_message>
<xml_diff>
--- a/inst/extdata/Testing new_R_ps/new_R_ps_example.xlsx
+++ b/inst/extdata/Testing new_R_ps/new_R_ps_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/Recca/inst/extdata/Testing new_R_ps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117E5643-9A40-5243-BC06-36C048CEEC92}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EA3BBD-4910-544E-99FC-A9F2EBB08175}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -951,7 +951,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1255" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="180">
   <si>
     <t>Buildings</t>
   </si>
@@ -3892,32 +3892,7 @@
     <t>g_rev' = L_ixp_rev * y_rev'</t>
   </si>
   <si>
-    <t>g_rev_hat'</t>
-  </si>
-  <si>
-    <r>
-      <t>U_rev' = Z_rev * g_rev_hat</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>'</t>
-    </r>
-  </si>
-  <si>
-    <t>V_rev' = D_rev * q_rev_hat'</t>
-  </si>
-  <si>
-    <t>R_rev' = (R_rev * q_rev_hat_inv) * q_rev_hat'</t>
-  </si>
-  <si>
     <t>q_rev' = L_pxp_rev * y_rev'</t>
-  </si>
-  <si>
-    <t>q_rev_hat'</t>
   </si>
   <si>
     <r>
@@ -4182,50 +4157,6 @@
   </si>
   <si>
     <r>
-      <t>D_rev</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>U</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>T</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>*q_hat_inv</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Z_rev</t>
     </r>
     <r>
@@ -4279,6 +4210,339 @@
       </rPr>
       <t>f_hat_inv</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t>L_pxp_rev</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A_rev</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>D_rev</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>U</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>q_hat_inv</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L_ixp_rev = D_rev</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>L_pxp_rev</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>g_rev' = L_ixp_rev</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> * (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>q_rev'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>L_pxp_rev</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> * (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>g_rev'_hat</t>
+  </si>
+  <si>
+    <t>q_rev'_hat</t>
+  </si>
+  <si>
+    <t>V_rev' = D_rev * q_rev'_hat</t>
+  </si>
+  <si>
+    <t>R_rev' = (R_rev * q_rev_hat_inv) * q_rev'_hat</t>
+  </si>
+  <si>
+    <t>U_rev' = Z_rev * g_rev'_hat</t>
   </si>
 </sst>
 </file>
@@ -36964,8 +37228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5018262C-ADF6-FA4F-AD02-C6E8C0BF89C2}">
   <dimension ref="A1:GE147"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AI86" sqref="AI86:AP93"/>
+    <sheetView showGridLines="0" topLeftCell="BP37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="DV54" sqref="DV54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -40807,7 +41071,7 @@
         <v>156</v>
       </c>
       <c r="DV53" s="67" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="DW53" s="67"/>
       <c r="DX53" s="67"/>
@@ -40840,7 +41104,7 @@
       <c r="EV53" s="8"/>
       <c r="EW53" s="57"/>
       <c r="FM53" s="67" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="FN53" s="67"/>
       <c r="FO53" s="67"/>
@@ -40849,7 +41113,7 @@
       <c r="FR53" s="67"/>
       <c r="FS53" s="8"/>
       <c r="FT53" s="67" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="FU53" s="67"/>
       <c r="FW53" s="46" t="s">
@@ -42836,7 +43100,7 @@
         <v>157</v>
       </c>
       <c r="DB71" s="67" t="s">
-        <v>158</v>
+        <v>175</v>
       </c>
       <c r="DC71" s="67"/>
       <c r="DD71" s="67"/>
@@ -42849,7 +43113,7 @@
       <c r="DK71" s="8"/>
       <c r="DL71" s="8"/>
       <c r="DM71" s="67" t="s">
-        <v>160</v>
+        <v>177</v>
       </c>
       <c r="DN71" s="67"/>
       <c r="DO71" s="67"/>
@@ -42872,7 +43136,7 @@
       <c r="FB71" s="8"/>
       <c r="FC71" s="8"/>
       <c r="FD71" s="67" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="FE71" s="67"/>
       <c r="FF71" s="67"/>
@@ -43662,7 +43926,7 @@
       <c r="BL80" s="74"/>
       <c r="DL80" s="1"/>
       <c r="DM80" s="67" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="DN80" s="67"/>
       <c r="DO80" s="67"/>
@@ -43673,7 +43937,7 @@
       <c r="DT80" s="67"/>
       <c r="FC80" s="1"/>
       <c r="FD80" s="67" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="FE80" s="67"/>
       <c r="FF80" s="67"/>
@@ -46036,7 +46300,7 @@
       <c r="BC94" s="8"/>
       <c r="BD94" s="8"/>
       <c r="BE94" s="67" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="BF94" s="67"/>
       <c r="BG94" s="67"/>
@@ -46072,10 +46336,10 @@
       <c r="CN94" s="8"/>
       <c r="CO94" s="57"/>
       <c r="CX94" s="46" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="DB94" s="67" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="DC94" s="67"/>
       <c r="DD94" s="67"/>
@@ -46086,7 +46350,7 @@
       <c r="DI94" s="67"/>
       <c r="DJ94" s="8"/>
       <c r="DV94" s="75" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="DW94" s="75"/>
       <c r="DX94" s="75"/>
@@ -46370,7 +46634,7 @@
       <c r="P98" s="75"/>
       <c r="Q98" s="75"/>
       <c r="DV98" s="75" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="DW98" s="75"/>
       <c r="DX98" s="75"/>
@@ -47561,10 +47825,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DK144"/>
+  <dimension ref="A1:EV144"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BU45" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="DD83" sqref="DD83:DK90"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="EO92" sqref="EO92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -47918,7 +48182,7 @@
       <c r="G30" s="14"/>
       <c r="CQ30" s="1"/>
       <c r="CR30" s="67" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="CS30" s="67"/>
       <c r="CT30" s="67"/>
@@ -50158,7 +50422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:150" x14ac:dyDescent="0.2">
       <c r="A49" s="69"/>
       <c r="B49" s="1" t="s">
         <v>18</v>
@@ -50395,7 +50659,7 @@
         <v>0.20996441281138789</v>
       </c>
     </row>
-    <row r="50" spans="1:115" ht="19" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:150" ht="19" x14ac:dyDescent="0.2">
       <c r="B50" s="1"/>
       <c r="L50" s="67" t="s">
         <v>2</v>
@@ -50477,17 +50741,17 @@
       <c r="CN50" s="80"/>
       <c r="CO50" s="8"/>
       <c r="CS50" s="67" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="CT50" s="67"/>
       <c r="CU50" s="82"/>
       <c r="CV50" s="82" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="DB50" s="31"/>
       <c r="DC50" s="84"/>
       <c r="DD50" s="67" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="DE50" s="67"/>
       <c r="DF50" s="67"/>
@@ -50495,7 +50759,7 @@
       <c r="DH50" s="67"/>
       <c r="DI50" s="67"/>
     </row>
-    <row r="51" spans="1:115" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:150" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="1"/>
       <c r="J51" s="69" t="s">
         <v>30</v>
@@ -50556,7 +50820,7 @@
       <c r="DD51" s="31"/>
       <c r="DE51" s="31"/>
     </row>
-    <row r="52" spans="1:115" ht="17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:150" ht="17" x14ac:dyDescent="0.2">
       <c r="B52" s="1"/>
       <c r="J52" s="69"/>
       <c r="K52" s="37" t="s">
@@ -50586,7 +50850,7 @@
       <c r="Z52" s="59"/>
       <c r="AB52" s="59"/>
     </row>
-    <row r="53" spans="1:115" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:150" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" s="1"/>
       <c r="J53" s="69"/>
       <c r="K53" s="1" t="s">
@@ -50621,7 +50885,7 @@
       <c r="Z53" s="15"/>
       <c r="AA53" s="15"/>
     </row>
-    <row r="54" spans="1:115" ht="20" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:150" ht="20" x14ac:dyDescent="0.25">
       <c r="L54" s="71" t="s">
         <v>42</v>
       </c>
@@ -50631,7 +50895,7 @@
       <c r="P54" s="71"/>
       <c r="Q54" s="71"/>
     </row>
-    <row r="55" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:150" x14ac:dyDescent="0.2">
       <c r="L55" s="6">
         <f t="shared" ref="L55:Q55" si="8">SUM(L51:L53)</f>
         <v>100</v>
@@ -50657,7 +50921,7 @@
         <v>28.1</v>
       </c>
     </row>
-    <row r="56" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:150" x14ac:dyDescent="0.2">
       <c r="L56" s="67" t="s">
         <v>86</v>
       </c>
@@ -50667,7 +50931,7 @@
       <c r="P56" s="67"/>
       <c r="Q56" s="67"/>
     </row>
-    <row r="59" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:150" x14ac:dyDescent="0.2">
       <c r="CQ59" s="31"/>
       <c r="CR59" s="31"/>
       <c r="CS59" s="31"/>
@@ -50679,7 +50943,7 @@
       <c r="CY59" s="31"/>
       <c r="CZ59" s="31"/>
     </row>
-    <row r="60" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:150" x14ac:dyDescent="0.2">
       <c r="B60" s="1"/>
       <c r="Z60" s="68" t="s">
         <v>30</v>
@@ -50742,8 +51006,18 @@
       <c r="DI60" s="67"/>
       <c r="DJ60" s="67"/>
       <c r="DK60" s="67"/>
+      <c r="EA60" s="67" t="s">
+        <v>4</v>
+      </c>
+      <c r="EB60" s="67"/>
+      <c r="EC60" s="67"/>
+      <c r="ED60" s="67"/>
+      <c r="EE60" s="67"/>
+      <c r="EF60" s="67"/>
+      <c r="EG60" s="67"/>
+      <c r="EH60" s="67"/>
     </row>
-    <row r="61" spans="1:115" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:150" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="1"/>
       <c r="V61" s="60"/>
       <c r="W61" s="60"/>
@@ -50874,8 +51148,32 @@
       <c r="DK61" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="EA61" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="EB61" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="EC61" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="ED61" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="EE61" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="EF61" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="EG61" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="EH61" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="62" spans="1:115" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:150" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="69" t="s">
         <v>3</v>
       </c>
@@ -51083,8 +51381,68 @@
         <f ca="1"/>
         <v>0</v>
       </c>
+      <c r="EA62" s="6">
+        <f t="array" aca="1" ref="EA62:EH67" ca="1">MMULT(DD62:DK67, EA83:EH90)</f>
+        <v>1.0309278350515463</v>
+      </c>
+      <c r="EB62" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EC62" s="6">
+        <f ca="1"/>
+        <v>0.13807069219440354</v>
+      </c>
+      <c r="ED62" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EE62" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EF62" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EG62" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EH62" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EK62" s="6">
+        <f t="array" aca="1" ref="EK62:EK67" ca="1">MMULT(EA62:EH67, CV42:CV49)</f>
+        <v>99.999999999999986</v>
+      </c>
+      <c r="EO62" s="6">
+        <f ca="1">IF((ROW()-ROW($EO$62))=(COLUMN()-COLUMN($EO$62)),INDIRECT("EK"&amp;ROW()),0)</f>
+        <v>99.999999999999986</v>
+      </c>
+      <c r="EP62" s="6">
+        <f t="shared" ref="EP62:ET67" ca="1" si="13">IF((ROW()-ROW($EO$62))=(COLUMN()-COLUMN($EO$62)),INDIRECT("EK"&amp;ROW()),0)</f>
+        <v>0</v>
+      </c>
+      <c r="EQ62" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="ER62" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="ES62" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="ET62" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="63" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:150" x14ac:dyDescent="0.2">
       <c r="A63" s="69"/>
       <c r="B63" s="1" t="s">
         <v>24</v>
@@ -51289,8 +51647,68 @@
         <f ca="1"/>
         <v>0</v>
       </c>
+      <c r="EA63" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EB63" s="6">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="EC63" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="ED63" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EE63" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EF63" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EG63" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EH63" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EK63" s="6">
+        <f ca="1"/>
+        <v>87</v>
+      </c>
+      <c r="EO63" s="6">
+        <f t="shared" ref="EO63:EO67" ca="1" si="14">IF((ROW()-ROW($EO$62))=(COLUMN()-COLUMN($EO$62)),INDIRECT("EK"&amp;ROW()),0)</f>
+        <v>0</v>
+      </c>
+      <c r="EP63" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>87</v>
+      </c>
+      <c r="EQ63" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="ER63" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="ES63" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="ET63" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="64" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:150" x14ac:dyDescent="0.2">
       <c r="A64" s="69"/>
       <c r="B64" s="1" t="s">
         <v>25</v>
@@ -51495,8 +51913,68 @@
         <f ca="1"/>
         <v>0</v>
       </c>
+      <c r="EA64" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EB64" s="6">
+        <f ca="1"/>
+        <v>0.20459770114942533</v>
+      </c>
+      <c r="EC64" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="ED64" s="6">
+        <f ca="1"/>
+        <v>0.22762148337595911</v>
+      </c>
+      <c r="EE64" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EF64" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EG64" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EH64" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EK64" s="6">
+        <f ca="1"/>
+        <v>17.800000000000004</v>
+      </c>
+      <c r="EO64" s="6">
+        <f t="shared" ca="1" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="EP64" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="EQ64" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>17.800000000000004</v>
+      </c>
+      <c r="ER64" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="ES64" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="ET64" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="65" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:150" x14ac:dyDescent="0.2">
       <c r="A65" s="69"/>
       <c r="B65" s="1" t="s">
         <v>0</v>
@@ -51701,8 +52179,68 @@
         <f ca="1"/>
         <v>0</v>
       </c>
+      <c r="EA65" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EB65" s="6">
+        <f ca="1"/>
+        <v>0.51034482758620692</v>
+      </c>
+      <c r="EC65" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="ED65" s="6">
+        <f ca="1"/>
+        <v>0.56777493606138107</v>
+      </c>
+      <c r="EE65" s="6">
+        <f ca="1"/>
+        <v>0.96031746031746024</v>
+      </c>
+      <c r="EF65" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EG65" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EH65" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EK65" s="6">
+        <f ca="1"/>
+        <v>44.4</v>
+      </c>
+      <c r="EO65" s="6">
+        <f t="shared" ca="1" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="EP65" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="EQ65" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="ER65" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>44.4</v>
+      </c>
+      <c r="ES65" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="ET65" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="66" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:150" x14ac:dyDescent="0.2">
       <c r="A66" s="69"/>
       <c r="B66" s="1" t="s">
         <v>15</v>
@@ -51907,8 +52445,68 @@
         <f ca="1"/>
         <v>0</v>
       </c>
+      <c r="EA66" s="6">
+        <f ca="1"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="EB66" s="6">
+        <f ca="1"/>
+        <v>5.7471264367816109E-3</v>
+      </c>
+      <c r="EC66" s="6">
+        <f ca="1"/>
+        <v>0.8928571428571429</v>
+      </c>
+      <c r="ED66" s="6">
+        <f ca="1"/>
+        <v>6.3938618925831209E-3</v>
+      </c>
+      <c r="EE66" s="6">
+        <f ca="1"/>
+        <v>3.968253968253968E-2</v>
+      </c>
+      <c r="EF66" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EG66" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EH66" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EK66" s="6">
+        <f ca="1"/>
+        <v>19.899999999999995</v>
+      </c>
+      <c r="EO66" s="6">
+        <f t="shared" ca="1" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="EP66" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="EQ66" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="ER66" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="ES66" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>19.899999999999995</v>
+      </c>
+      <c r="ET66" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="67" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:150" x14ac:dyDescent="0.2">
       <c r="A67" s="69"/>
       <c r="B67" s="1" t="s">
         <v>16</v>
@@ -52113,8 +52711,68 @@
         <f ca="1"/>
         <v>0</v>
       </c>
+      <c r="EA67" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EB67" s="6">
+        <f ca="1"/>
+        <v>0.32298850574712651</v>
+      </c>
+      <c r="EC67" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="ED67" s="6">
+        <f ca="1"/>
+        <v>0.35933503836317143</v>
+      </c>
+      <c r="EE67" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EF67" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EG67" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EH67" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EK67" s="6">
+        <f ca="1"/>
+        <v>28.100000000000005</v>
+      </c>
+      <c r="EO67" s="6">
+        <f t="shared" ca="1" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="EP67" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="EQ67" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="ER67" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="ES67" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="ET67" s="6">
+        <f t="shared" ca="1" si="13"/>
+        <v>28.100000000000005</v>
+      </c>
     </row>
-    <row r="68" spans="1:115" ht="20" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:150" ht="20" x14ac:dyDescent="0.25">
       <c r="C68" s="67" t="s">
         <v>5</v>
       </c>
@@ -52197,7 +52855,7 @@
       <c r="CY68" s="63"/>
       <c r="CZ68" s="63"/>
       <c r="DD68" s="73" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="DE68" s="73"/>
       <c r="DF68" s="73"/>
@@ -52206,38 +52864,59 @@
       <c r="DI68" s="73"/>
       <c r="DJ68" s="73"/>
       <c r="DK68" s="73"/>
+      <c r="EA68" s="70" t="s">
+        <v>172</v>
+      </c>
+      <c r="EB68" s="70"/>
+      <c r="EC68" s="70"/>
+      <c r="ED68" s="70"/>
+      <c r="EE68" s="70"/>
+      <c r="EF68" s="70"/>
+      <c r="EG68" s="70"/>
+      <c r="EH68" s="70"/>
+      <c r="EK68" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="EO68" s="67" t="s">
+        <v>175</v>
+      </c>
+      <c r="EP68" s="67"/>
+      <c r="EQ68" s="67"/>
+      <c r="ER68" s="67"/>
+      <c r="ES68" s="67"/>
+      <c r="ET68" s="67"/>
     </row>
-    <row r="69" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:150" x14ac:dyDescent="0.2">
       <c r="C69" s="20">
         <f>SUM(C62:C67)</f>
         <v>0</v>
       </c>
       <c r="D69" s="20">
-        <f t="shared" ref="D69:J69" si="13">SUM(D62:D67)</f>
+        <f t="shared" ref="D69:J69" si="15">SUM(D62:D67)</f>
         <v>0</v>
       </c>
       <c r="E69" s="20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>22.4</v>
       </c>
       <c r="F69" s="20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>78.2</v>
       </c>
       <c r="G69" s="20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>12.6</v>
       </c>
       <c r="H69" s="20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>25.2</v>
       </c>
       <c r="I69" s="20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.4</v>
       </c>
       <c r="J69" s="20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>5.9</v>
       </c>
       <c r="X69" s="15"/>
@@ -52295,7 +52974,7 @@
       <c r="CY69" s="63"/>
       <c r="CZ69" s="63"/>
     </row>
-    <row r="70" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:150" x14ac:dyDescent="0.2">
       <c r="C70" s="67" t="s">
         <v>73</v>
       </c>
@@ -52361,7 +53040,7 @@
       <c r="CY70" s="74"/>
       <c r="CZ70" s="74"/>
     </row>
-    <row r="71" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:150" x14ac:dyDescent="0.2">
       <c r="CQ71" s="31"/>
       <c r="CR71" s="31"/>
       <c r="CS71" s="63"/>
@@ -52373,7 +53052,7 @@
       <c r="CY71" s="63"/>
       <c r="CZ71" s="63"/>
     </row>
-    <row r="72" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:150" x14ac:dyDescent="0.2">
       <c r="CQ72" s="31"/>
       <c r="CR72" s="31"/>
       <c r="CS72" s="71"/>
@@ -52385,7 +53064,7 @@
       <c r="CY72" s="71"/>
       <c r="CZ72" s="71"/>
     </row>
-    <row r="73" spans="1:115" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:150" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B73" s="1"/>
       <c r="L73" s="63"/>
       <c r="M73" s="63"/>
@@ -52429,7 +53108,7 @@
       <c r="AZ73" s="67"/>
       <c r="BA73" s="67"/>
     </row>
-    <row r="74" spans="1:115" ht="87" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:150" ht="87" x14ac:dyDescent="0.2">
       <c r="B74" s="1"/>
       <c r="L74" s="63"/>
       <c r="M74" s="63"/>
@@ -52494,7 +53173,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:115" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:150" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="69" t="s">
         <v>84</v>
       </c>
@@ -52604,7 +53283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:150" x14ac:dyDescent="0.2">
       <c r="A76" s="69"/>
       <c r="B76" s="1" t="s">
         <v>21</v>
@@ -52711,7 +53390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:115" ht="18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:150" ht="18" x14ac:dyDescent="0.25">
       <c r="B77" s="1"/>
       <c r="C77" s="67" t="s">
         <v>51</v>
@@ -52768,38 +53447,38 @@
       <c r="AZ77" s="74"/>
       <c r="BA77" s="74"/>
     </row>
-    <row r="78" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:150" x14ac:dyDescent="0.2">
       <c r="B78" s="1"/>
       <c r="C78" s="6">
         <f>SUM(C75:C76)</f>
         <v>97</v>
       </c>
       <c r="D78" s="6">
-        <f t="shared" ref="D78:J78" si="14">SUM(D75:D76)</f>
+        <f t="shared" ref="D78:J78" si="16">SUM(D75:D76)</f>
         <v>87</v>
       </c>
       <c r="E78" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="F78" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="G78" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H78" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="I78" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="J78" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="L78" s="63"/>
@@ -52819,7 +53498,7 @@
       <c r="Z78" s="62"/>
       <c r="AA78" s="62"/>
     </row>
-    <row r="79" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:150" x14ac:dyDescent="0.2">
       <c r="C79" s="67" t="s">
         <v>54</v>
       </c>
@@ -52831,41 +53510,41 @@
       <c r="I79" s="67"/>
       <c r="J79" s="67"/>
     </row>
-    <row r="80" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:150" x14ac:dyDescent="0.2">
       <c r="C80" s="6">
         <f>C78+SUM(C62:C67)</f>
         <v>97</v>
       </c>
       <c r="D80" s="6">
-        <f t="shared" ref="D80:J80" si="15">D78+SUM(D62:D67)</f>
+        <f t="shared" ref="D80:J80" si="17">D78+SUM(D62:D67)</f>
         <v>87</v>
       </c>
       <c r="E80" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>22.4</v>
       </c>
       <c r="F80" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>78.2</v>
       </c>
       <c r="G80" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>12.6</v>
       </c>
       <c r="H80" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>25.2</v>
       </c>
       <c r="I80" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0.4</v>
       </c>
       <c r="J80" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>5.9</v>
       </c>
     </row>
-    <row r="81" spans="1:115" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:152" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C81" s="75" t="s">
         <v>85</v>
       </c>
@@ -52924,8 +53603,28 @@
       <c r="DI81" s="67"/>
       <c r="DJ81" s="67"/>
       <c r="DK81" s="67"/>
+      <c r="DP81" s="67" t="s">
+        <v>4</v>
+      </c>
+      <c r="DQ81" s="67"/>
+      <c r="DR81" s="67"/>
+      <c r="DS81" s="67"/>
+      <c r="DT81" s="67"/>
+      <c r="DU81" s="67"/>
+      <c r="DV81" s="67"/>
+      <c r="DW81" s="67"/>
+      <c r="EA81" s="67" t="s">
+        <v>4</v>
+      </c>
+      <c r="EB81" s="67"/>
+      <c r="EC81" s="67"/>
+      <c r="ED81" s="67"/>
+      <c r="EE81" s="67"/>
+      <c r="EF81" s="67"/>
+      <c r="EG81" s="67"/>
+      <c r="EH81" s="67"/>
     </row>
-    <row r="82" spans="1:115" ht="114" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:152" ht="114" x14ac:dyDescent="0.2">
       <c r="AI82" s="2" t="s">
         <v>23</v>
       </c>
@@ -53040,8 +53739,56 @@
       <c r="DK82" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="DP82" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="DQ82" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="DR82" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="DS82" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="DT82" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="DU82" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="DV82" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="DW82" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="EA82" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="EB82" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="EC82" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="ED82" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="EE82" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="EF82" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="EG82" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="EH82" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="83" spans="1:115" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:152" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="69" t="s">
         <v>4</v>
       </c>
@@ -53068,7 +53815,7 @@
         <v>0</v>
       </c>
       <c r="Z83" s="6">
-        <f t="shared" ref="Z83:Z90" si="16">SUM(L83:Q83)</f>
+        <f t="shared" ref="Z83:Z90" si="18">SUM(L83:Q83)</f>
         <v>-97</v>
       </c>
       <c r="AI83" s="6">
@@ -53172,7 +53919,7 @@
         <v>97.000000000000014</v>
       </c>
       <c r="BP83" s="7">
-        <f t="shared" ref="BP83:BP90" ca="1" si="17">BO83-AB42</f>
+        <f t="shared" ref="BP83:BP90" ca="1" si="19">BO83-AB42</f>
         <v>0</v>
       </c>
       <c r="BT83" s="6">
@@ -53200,7 +53947,7 @@
         <v>0</v>
       </c>
       <c r="CA83" s="7">
-        <f t="shared" ref="CA83:CA90" ca="1" si="18">SUM(BT83:BY83)</f>
+        <f t="shared" ref="CA83:CA90" ca="1" si="20">SUM(BT83:BY83)</f>
         <v>1</v>
       </c>
       <c r="CQ83" s="69" t="s">
@@ -53241,8 +53988,108 @@
         <f ca="1"/>
         <v>0</v>
       </c>
+      <c r="DP83" s="6">
+        <f t="array" aca="1" ref="DP83:DW90" ca="1">_xlfn.MUNIT(8) - DD83:DK90</f>
+        <v>1</v>
+      </c>
+      <c r="DQ83" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DR83" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DS83" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DT83" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DU83" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DV83" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DW83" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EA83" s="6">
+        <f t="array" aca="1" ref="EA83:EH90" ca="1">MINVERSE(DP83:DW90)</f>
+        <v>1</v>
+      </c>
+      <c r="EB83" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EC83" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="ED83" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EE83" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EF83" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EG83" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EH83" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EK83" s="6">
+        <f t="array" aca="1" ref="EK83:EK90" ca="1">MMULT(EA83:EH90, CV42:CV49)</f>
+        <v>97</v>
+      </c>
+      <c r="EO83" s="6">
+        <f ca="1">IF((ROW()-ROW($EO$83))=(COLUMN()-COLUMN($EO$83)),INDIRECT("EK"&amp;ROW()),0)</f>
+        <v>97</v>
+      </c>
+      <c r="EP83" s="6">
+        <f t="shared" ref="EP83:EV90" ca="1" si="21">IF((ROW()-ROW($EO$83))=(COLUMN()-COLUMN($EO$83)),INDIRECT("EK"&amp;ROW()),0)</f>
+        <v>0</v>
+      </c>
+      <c r="EQ83" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="ER83" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="ES83" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="ET83" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="EU83" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="EV83" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="84" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:152" x14ac:dyDescent="0.2">
       <c r="A84" s="69"/>
       <c r="B84" s="1" t="s">
         <v>1</v>
@@ -53266,7 +54113,7 @@
         <v>0</v>
       </c>
       <c r="Z84" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>-87</v>
       </c>
       <c r="AI84" s="6">
@@ -53370,7 +54217,7 @@
         <v>87</v>
       </c>
       <c r="BP84" s="7">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="19"/>
         <v>0</v>
       </c>
       <c r="BT84" s="6">
@@ -53398,7 +54245,7 @@
         <v>0</v>
       </c>
       <c r="CA84" s="7">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="20"/>
         <v>1</v>
       </c>
       <c r="CQ84" s="69"/>
@@ -53437,8 +54284,108 @@
         <f ca="1"/>
         <v>0</v>
       </c>
+      <c r="DP84" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DQ84" s="6">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="DR84" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DS84" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DT84" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DU84" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DV84" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DW84" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EA84" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EB84" s="6">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="EC84" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="ED84" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EE84" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EF84" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EG84" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EH84" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EK84" s="6">
+        <f ca="1"/>
+        <v>87</v>
+      </c>
+      <c r="EO84" s="6">
+        <f t="shared" ref="EO84:EO90" ca="1" si="22">IF((ROW()-ROW($EO$83))=(COLUMN()-COLUMN($EO$83)),INDIRECT("EK"&amp;ROW()),0)</f>
+        <v>0</v>
+      </c>
+      <c r="EP84" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>87</v>
+      </c>
+      <c r="EQ84" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="ER84" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="ES84" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="ET84" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="EU84" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="EV84" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="85" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:152" x14ac:dyDescent="0.2">
       <c r="A85" s="69"/>
       <c r="B85" s="1" t="s">
         <v>27</v>
@@ -53462,7 +54409,7 @@
         <v>0</v>
       </c>
       <c r="Z85" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AI85" s="6">
@@ -53566,7 +54513,7 @@
         <v>22.400000000000002</v>
       </c>
       <c r="BP85" s="7">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="19"/>
         <v>0</v>
       </c>
       <c r="BT85" s="6">
@@ -53594,7 +54541,7 @@
         <v>0</v>
       </c>
       <c r="CA85" s="7">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="20"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="CQ85" s="69"/>
@@ -53633,8 +54580,108 @@
         <f ca="1"/>
         <v>0</v>
       </c>
+      <c r="DP85" s="6">
+        <f ca="1"/>
+        <v>-0.22399999999999998</v>
+      </c>
+      <c r="DQ85" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DR85" s="6">
+        <f ca="1"/>
+        <v>0.97</v>
+      </c>
+      <c r="DS85" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DT85" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DU85" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DV85" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DW85" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EA85" s="6">
+        <f ca="1"/>
+        <v>0.23092783505154638</v>
+      </c>
+      <c r="EB85" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EC85" s="6">
+        <f ca="1"/>
+        <v>1.0309278350515465</v>
+      </c>
+      <c r="ED85" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EE85" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EF85" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EG85" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EH85" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EK85" s="6">
+        <f ca="1"/>
+        <v>22.4</v>
+      </c>
+      <c r="EO85" s="6">
+        <f t="shared" ca="1" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="EP85" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="EQ85" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>22.4</v>
+      </c>
+      <c r="ER85" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="ES85" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="ET85" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="EU85" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="EV85" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="86" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:152" x14ac:dyDescent="0.2">
       <c r="A86" s="69"/>
       <c r="B86" s="1" t="s">
         <v>26</v>
@@ -53658,7 +54705,7 @@
         <v>-28.1</v>
       </c>
       <c r="Z86" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AI86" s="6">
@@ -53762,7 +54809,7 @@
         <v>78.199999999999989</v>
       </c>
       <c r="BP86" s="7">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="19"/>
         <v>0</v>
       </c>
       <c r="BT86" s="6">
@@ -53790,7 +54837,7 @@
         <v>0.35933503836317143</v>
       </c>
       <c r="CA86" s="7">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="20"/>
         <v>1.0000000000000002</v>
       </c>
       <c r="CQ86" s="69"/>
@@ -53829,8 +54876,108 @@
         <f ca="1"/>
         <v>0</v>
       </c>
+      <c r="DP86" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DQ86" s="6">
+        <f ca="1"/>
+        <v>-0.89885057471264374</v>
+      </c>
+      <c r="DR86" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DS86" s="6">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="DT86" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DU86" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DV86" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DW86" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EA86" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EB86" s="6">
+        <f ca="1"/>
+        <v>0.89885057471264374</v>
+      </c>
+      <c r="EC86" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="ED86" s="6">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="EE86" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EF86" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EG86" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EH86" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EK86" s="6">
+        <f ca="1"/>
+        <v>78.2</v>
+      </c>
+      <c r="EO86" s="6">
+        <f t="shared" ca="1" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="EP86" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="EQ86" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="ER86" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>78.2</v>
+      </c>
+      <c r="ES86" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="ET86" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="EU86" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="EV86" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="87" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:152" x14ac:dyDescent="0.2">
       <c r="A87" s="69"/>
       <c r="B87" s="1" t="s">
         <v>29</v>
@@ -53854,7 +55001,7 @@
         <v>0</v>
       </c>
       <c r="Z87" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AI87" s="6">
@@ -53958,7 +55105,7 @@
         <v>12.599999999999998</v>
       </c>
       <c r="BP87" s="7">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="19"/>
         <v>0</v>
       </c>
       <c r="BT87" s="6">
@@ -53986,7 +55133,7 @@
         <v>0</v>
       </c>
       <c r="CA87" s="7">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="20"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="CQ87" s="69"/>
@@ -54025,8 +55172,108 @@
         <f ca="1"/>
         <v>0</v>
       </c>
+      <c r="DP87" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DQ87" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DR87" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DS87" s="6">
+        <f ca="1"/>
+        <v>-0.16112531969309465</v>
+      </c>
+      <c r="DT87" s="6">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="DU87" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DV87" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DW87" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EA87" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EB87" s="6">
+        <f ca="1"/>
+        <v>0.14482758620689659</v>
+      </c>
+      <c r="EC87" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="ED87" s="6">
+        <f ca="1"/>
+        <v>0.16112531969309465</v>
+      </c>
+      <c r="EE87" s="6">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="EF87" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EG87" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EH87" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EK87" s="6">
+        <f ca="1"/>
+        <v>12.600000000000003</v>
+      </c>
+      <c r="EO87" s="6">
+        <f t="shared" ca="1" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="EP87" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="EQ87" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="ER87" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="ES87" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>12.600000000000003</v>
+      </c>
+      <c r="ET87" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="EU87" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="EV87" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="88" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:152" x14ac:dyDescent="0.2">
       <c r="A88" s="69"/>
       <c r="B88" s="1" t="s">
         <v>19</v>
@@ -54050,7 +55297,7 @@
         <v>0</v>
       </c>
       <c r="Z88" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>25.2</v>
       </c>
       <c r="AI88" s="6">
@@ -54154,7 +55401,7 @@
         <v>25.2</v>
       </c>
       <c r="BP88" s="7">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="19"/>
         <v>0</v>
       </c>
       <c r="BT88" s="6">
@@ -54182,7 +55429,7 @@
         <v>0</v>
       </c>
       <c r="CA88" s="7">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="20"/>
         <v>0</v>
       </c>
       <c r="CQ88" s="69"/>
@@ -54221,8 +55468,108 @@
         <f ca="1"/>
         <v>0</v>
       </c>
+      <c r="DP88" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DQ88" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DR88" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DS88" s="6">
+        <f ca="1"/>
+        <v>-0.23443008225616924</v>
+      </c>
+      <c r="DT88" s="6">
+        <f ca="1"/>
+        <v>-0.54504504504504503</v>
+      </c>
+      <c r="DU88" s="6">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="DV88" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DW88" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EA88" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EB88" s="6">
+        <f ca="1"/>
+        <v>0.28965517241379313</v>
+      </c>
+      <c r="EC88" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="ED88" s="6">
+        <f ca="1"/>
+        <v>0.32225063938618931</v>
+      </c>
+      <c r="EE88" s="6">
+        <f ca="1"/>
+        <v>0.54504504504504503</v>
+      </c>
+      <c r="EF88" s="6">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="EG88" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EH88" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EK88" s="6">
+        <f ca="1"/>
+        <v>25.200000000000003</v>
+      </c>
+      <c r="EO88" s="6">
+        <f t="shared" ca="1" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="EP88" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="EQ88" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="ER88" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="ES88" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="ET88" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>25.200000000000003</v>
+      </c>
+      <c r="EU88" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="EV88" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="89" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:152" x14ac:dyDescent="0.2">
       <c r="A89" s="69"/>
       <c r="B89" s="1" t="s">
         <v>17</v>
@@ -54246,7 +55593,7 @@
         <v>0</v>
       </c>
       <c r="Z89" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.4</v>
       </c>
       <c r="AI89" s="6">
@@ -54350,7 +55697,7 @@
         <v>0.4</v>
       </c>
       <c r="BP89" s="7">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="19"/>
         <v>0</v>
       </c>
       <c r="BT89" s="6">
@@ -54378,7 +55725,7 @@
         <v>0</v>
       </c>
       <c r="CA89" s="7">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="20"/>
         <v>0</v>
       </c>
       <c r="CQ89" s="69"/>
@@ -54417,8 +55764,108 @@
         <f ca="1"/>
         <v>0</v>
       </c>
+      <c r="DP89" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DQ89" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DR89" s="6">
+        <f ca="1"/>
+        <v>-1.7408470926058867E-2</v>
+      </c>
+      <c r="DS89" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DT89" s="6">
+        <f ca="1"/>
+        <v>-7.9763898859376255E-4</v>
+      </c>
+      <c r="DU89" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DV89" s="6">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="DW89" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EA89" s="6">
+        <f ca="1"/>
+        <v>4.0201005025125632E-3</v>
+      </c>
+      <c r="EB89" s="6">
+        <f ca="1"/>
+        <v>1.1552012938254495E-4</v>
+      </c>
+      <c r="EC89" s="6">
+        <f ca="1"/>
+        <v>1.7946877243359659E-2</v>
+      </c>
+      <c r="ED89" s="6">
+        <f ca="1"/>
+        <v>1.2851983703684666E-4</v>
+      </c>
+      <c r="EE89" s="6">
+        <f ca="1"/>
+        <v>7.9763898859376255E-4</v>
+      </c>
+      <c r="EF89" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EG89" s="6">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="EH89" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EK89" s="6">
+        <f ca="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="EO89" s="6">
+        <f t="shared" ca="1" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="EP89" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="EQ89" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="ER89" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="ES89" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="ET89" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="EU89" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0.4</v>
+      </c>
+      <c r="EV89" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="90" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:152" x14ac:dyDescent="0.2">
       <c r="A90" s="69"/>
       <c r="B90" s="1" t="s">
         <v>18</v>
@@ -54442,7 +55889,7 @@
         <v>5.9</v>
       </c>
       <c r="Z90" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>5.9</v>
       </c>
       <c r="AI90" s="6">
@@ -54546,7 +55993,7 @@
         <v>5.9</v>
       </c>
       <c r="BP90" s="7">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="19"/>
         <v>0</v>
       </c>
       <c r="BT90" s="6">
@@ -54574,7 +56021,7 @@
         <v>0</v>
       </c>
       <c r="CA90" s="7">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="20"/>
         <v>0</v>
       </c>
       <c r="CQ90" s="69"/>
@@ -54613,8 +56060,108 @@
         <f ca="1"/>
         <v>0</v>
       </c>
+      <c r="DP90" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DQ90" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DR90" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DS90" s="6">
+        <f ca="1"/>
+        <v>-7.5447570332480826E-2</v>
+      </c>
+      <c r="DT90" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DU90" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DV90" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="DW90" s="6">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="EA90" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EB90" s="6">
+        <f ca="1"/>
+        <v>6.7816091954022995E-2</v>
+      </c>
+      <c r="EC90" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="ED90" s="6">
+        <f ca="1"/>
+        <v>7.5447570332480826E-2</v>
+      </c>
+      <c r="EE90" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EF90" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EG90" s="6">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="EH90" s="6">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="EK90" s="6">
+        <f ca="1"/>
+        <v>5.9</v>
+      </c>
+      <c r="EO90" s="6">
+        <f t="shared" ca="1" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="EP90" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="EQ90" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="ER90" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="ES90" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="ET90" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="EU90" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="EV90" s="6">
+        <f t="shared" ca="1" si="21"/>
+        <v>5.9</v>
+      </c>
     </row>
-    <row r="91" spans="1:115" ht="19" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:152" ht="19" x14ac:dyDescent="0.2">
       <c r="L91" s="75" t="s">
         <v>13</v>
       </c>
@@ -54698,8 +56245,41 @@
       <c r="DI91" s="67"/>
       <c r="DJ91" s="67"/>
       <c r="DK91" s="67"/>
+      <c r="DP91" s="67" t="s">
+        <v>142</v>
+      </c>
+      <c r="DQ91" s="67"/>
+      <c r="DR91" s="67"/>
+      <c r="DS91" s="67"/>
+      <c r="DT91" s="67"/>
+      <c r="DU91" s="67"/>
+      <c r="DV91" s="67"/>
+      <c r="DW91" s="67"/>
+      <c r="EA91" s="67" t="s">
+        <v>170</v>
+      </c>
+      <c r="EB91" s="67"/>
+      <c r="EC91" s="67"/>
+      <c r="ED91" s="67"/>
+      <c r="EE91" s="67"/>
+      <c r="EF91" s="67"/>
+      <c r="EG91" s="67"/>
+      <c r="EH91" s="67"/>
+      <c r="EK91" s="59" t="s">
+        <v>174</v>
+      </c>
+      <c r="EO91" s="67" t="s">
+        <v>176</v>
+      </c>
+      <c r="EP91" s="67"/>
+      <c r="EQ91" s="67"/>
+      <c r="ER91" s="67"/>
+      <c r="ES91" s="67"/>
+      <c r="ET91" s="67"/>
+      <c r="EU91" s="67"/>
+      <c r="EV91" s="67"/>
     </row>
-    <row r="92" spans="1:115" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:152" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J92" s="69" t="s">
         <v>30</v>
       </c>
@@ -54726,7 +56306,7 @@
         <v>-28.1</v>
       </c>
     </row>
-    <row r="93" spans="1:115" ht="17" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:152" ht="17" x14ac:dyDescent="0.2">
       <c r="J93" s="69"/>
       <c r="K93" s="37" t="s">
         <v>81</v>
@@ -54750,7 +56330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:152" x14ac:dyDescent="0.2">
       <c r="J94" s="69"/>
       <c r="K94" s="1" t="s">
         <v>33</v>
@@ -54784,7 +56364,7 @@
       <c r="Z94" s="17"/>
       <c r="AA94" s="17"/>
     </row>
-    <row r="95" spans="1:115" ht="20" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:152" ht="20" x14ac:dyDescent="0.25">
       <c r="L95" s="75" t="s">
         <v>35</v>
       </c>
@@ -54843,12 +56423,12 @@
         <v>97</v>
       </c>
       <c r="E102" s="6">
-        <f t="shared" ref="E102:E109" si="19">Z83</f>
+        <f t="shared" ref="E102:E109" si="23">Z83</f>
         <v>-97</v>
       </c>
       <c r="F102" s="63"/>
       <c r="G102" s="4">
-        <f t="shared" ref="G102:G109" si="20">Z42</f>
+        <f t="shared" ref="G102:G109" si="24">Z42</f>
         <v>0</v>
       </c>
       <c r="I102" s="7">
@@ -54865,16 +56445,16 @@
         <v>87</v>
       </c>
       <c r="E103" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>-87</v>
       </c>
       <c r="F103" s="63"/>
       <c r="G103" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="I103" s="7">
-        <f t="shared" ref="I103:I109" si="21">C103+E103-G103</f>
+        <f t="shared" ref="I103:I109" si="25">C103+E103-G103</f>
         <v>0</v>
       </c>
     </row>
@@ -54887,15 +56467,15 @@
         <v>0</v>
       </c>
       <c r="E104" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="G104" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="I104" s="7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
@@ -54911,21 +56491,21 @@
         <v>56</v>
       </c>
       <c r="E105" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="F105" s="59" t="s">
         <v>9</v>
       </c>
       <c r="G105" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="H105" s="60" t="s">
         <v>10</v>
       </c>
       <c r="I105" s="7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
@@ -54938,16 +56518,16 @@
         <v>0</v>
       </c>
       <c r="E106" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="F106" s="63"/>
       <c r="G106" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="I106" s="7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
@@ -54960,16 +56540,16 @@
         <v>0</v>
       </c>
       <c r="E107" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>25.2</v>
       </c>
       <c r="F107" s="63"/>
       <c r="G107" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>25.2</v>
       </c>
       <c r="I107" s="7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
@@ -54982,15 +56562,15 @@
         <v>0</v>
       </c>
       <c r="E108" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0.4</v>
       </c>
       <c r="G108" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0.4</v>
       </c>
       <c r="I108" s="7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
@@ -55003,16 +56583,16 @@
         <v>0</v>
       </c>
       <c r="E109" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>5.9</v>
       </c>
       <c r="F109" s="63"/>
       <c r="G109" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>5.9</v>
       </c>
       <c r="I109" s="7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
@@ -55100,11 +56680,11 @@
         <v>22.4</v>
       </c>
       <c r="D114" s="6">
-        <f t="shared" ref="D114:E119" si="22">AA62</f>
+        <f t="shared" ref="D114:E119" si="26">AA62</f>
         <v>0</v>
       </c>
       <c r="E114" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="G114" s="6">
@@ -55132,11 +56712,11 @@
         <v>0</v>
       </c>
       <c r="P114" s="7">
-        <f t="shared" ref="P114:Q119" si="23">D114-H114-L114</f>
+        <f t="shared" ref="P114:Q119" si="27">D114-H114-L114</f>
         <v>0</v>
       </c>
       <c r="Q114" s="7">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AO114" s="18"/>
@@ -55149,15 +56729,15 @@
         <v>24</v>
       </c>
       <c r="C115" s="6">
-        <f t="shared" ref="C115:C119" si="24">Z63</f>
+        <f t="shared" ref="C115:C119" si="28">Z63</f>
         <v>78.2</v>
       </c>
       <c r="D115" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="E115" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="G115" s="6">
@@ -55179,15 +56759,15 @@
         <v>0</v>
       </c>
       <c r="O115" s="7">
-        <f t="shared" ref="O115:O119" si="25">C115-G115-K115</f>
+        <f t="shared" ref="O115:O119" si="29">C115-G115-K115</f>
         <v>0</v>
       </c>
       <c r="P115" s="7">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="Q115" s="7">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AO115" s="18"/>
@@ -55200,15 +56780,15 @@
         <v>25</v>
       </c>
       <c r="C116" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>12.6</v>
       </c>
       <c r="D116" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="E116" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="F116" s="59" t="s">
@@ -55239,15 +56819,15 @@
         <v>10</v>
       </c>
       <c r="O116" s="7">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="P116" s="7">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="Q116" s="7">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AO116" s="18"/>
@@ -55260,15 +56840,15 @@
         <v>0</v>
       </c>
       <c r="C117" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="D117" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>25.2</v>
       </c>
       <c r="E117" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="G117" s="6">
@@ -55290,15 +56870,15 @@
         <v>0</v>
       </c>
       <c r="O117" s="7">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="P117" s="7">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="Q117" s="7">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AO117" s="18"/>
@@ -55311,15 +56891,15 @@
         <v>15</v>
       </c>
       <c r="C118" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="D118" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="E118" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0.4</v>
       </c>
       <c r="G118" s="6">
@@ -55341,15 +56921,15 @@
         <v>0</v>
       </c>
       <c r="O118" s="7">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="P118" s="7">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="Q118" s="7">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AO118" s="18"/>
@@ -55362,15 +56942,15 @@
         <v>16</v>
       </c>
       <c r="C119" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="D119" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="E119" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>5.9</v>
       </c>
       <c r="G119" s="6">
@@ -55392,15 +56972,15 @@
         <v>0</v>
       </c>
       <c r="O119" s="7">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="P119" s="7">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="Q119" s="7">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AO119" s="18"/>
@@ -55453,7 +57033,7 @@
         <v>22</v>
       </c>
       <c r="C125" s="6">
-        <f t="shared" ref="C125:C130" si="26">AD62</f>
+        <f t="shared" ref="C125:C130" si="30">AD62</f>
         <v>22.4</v>
       </c>
       <c r="D125" s="6">
@@ -55471,14 +57051,14 @@
         <v>24</v>
       </c>
       <c r="C126" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>78.2</v>
       </c>
       <c r="D126" s="6">
         <v>87</v>
       </c>
       <c r="F126" s="6">
-        <f t="shared" ref="F126:F130" si="27">C126/D126</f>
+        <f t="shared" ref="F126:F130" si="31">C126/D126</f>
         <v>0.89885057471264374</v>
       </c>
     </row>
@@ -55488,14 +57068,14 @@
         <v>25</v>
       </c>
       <c r="C127" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>12.6</v>
       </c>
       <c r="D127" s="6">
         <v>17.8</v>
       </c>
       <c r="F127" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>0.7078651685393258</v>
       </c>
     </row>
@@ -55505,14 +57085,14 @@
         <v>0</v>
       </c>
       <c r="C128" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>25.2</v>
       </c>
       <c r="D128" s="6">
         <v>44.4</v>
       </c>
       <c r="F128" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>0.56756756756756754</v>
       </c>
     </row>
@@ -55522,14 +57102,14 @@
         <v>15</v>
       </c>
       <c r="C129" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>0.4</v>
       </c>
       <c r="D129" s="6">
         <v>19.899999999999999</v>
       </c>
       <c r="F129" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>2.0100502512562818E-2</v>
       </c>
     </row>
@@ -55539,14 +57119,14 @@
         <v>16</v>
       </c>
       <c r="C130" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>5.9</v>
       </c>
       <c r="D130" s="6">
         <v>28.1</v>
       </c>
       <c r="F130" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>0.20996441281138789</v>
       </c>
     </row>
@@ -55604,27 +57184,27 @@
         <v>22</v>
       </c>
       <c r="C137" s="6">
-        <f t="shared" ref="C137:H142" ca="1" si="28">IF((ROW()-ROW($C$137))=(COLUMN()-COLUMN($C$137)),INDIRECT(ADDRESS(ROW(L$55),COLUMN(L$55))),0)</f>
+        <f t="shared" ref="C137:H142" ca="1" si="32">IF((ROW()-ROW($C$137))=(COLUMN()-COLUMN($C$137)),INDIRECT(ADDRESS(ROW(L$55),COLUMN(L$55))),0)</f>
         <v>100</v>
       </c>
       <c r="D137" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="E137" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="F137" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="G137" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="H137" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="J137" s="6">
@@ -55632,7 +57212,7 @@
         <v>22.4</v>
       </c>
       <c r="L137" s="7">
-        <f t="shared" ref="L137:L142" ca="1" si="29">J137-AD62</f>
+        <f t="shared" ref="L137:L142" ca="1" si="33">J137-AD62</f>
         <v>0</v>
       </c>
     </row>
@@ -55642,27 +57222,27 @@
         <v>24</v>
       </c>
       <c r="C138" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="D138" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>87</v>
       </c>
       <c r="E138" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="F138" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="G138" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="H138" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="J138" s="6">
@@ -55670,7 +57250,7 @@
         <v>78.2</v>
       </c>
       <c r="L138" s="7">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="33"/>
         <v>0</v>
       </c>
     </row>
@@ -55680,27 +57260,27 @@
         <v>25</v>
       </c>
       <c r="C139" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="D139" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="E139" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>17.8</v>
       </c>
       <c r="F139" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="G139" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="H139" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="J139" s="6">
@@ -55708,7 +57288,7 @@
         <v>12.6</v>
       </c>
       <c r="L139" s="7">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="33"/>
         <v>0</v>
       </c>
     </row>
@@ -55718,27 +57298,27 @@
         <v>0</v>
       </c>
       <c r="C140" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="D140" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="E140" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="F140" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>44.4</v>
       </c>
       <c r="G140" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="H140" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="J140" s="6">
@@ -55746,7 +57326,7 @@
         <v>25.2</v>
       </c>
       <c r="L140" s="7">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="33"/>
         <v>0</v>
       </c>
     </row>
@@ -55756,27 +57336,27 @@
         <v>15</v>
       </c>
       <c r="C141" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="D141" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="E141" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="F141" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="G141" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>19.899999999999999</v>
       </c>
       <c r="H141" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="J141" s="6">
@@ -55784,7 +57364,7 @@
         <v>0.4</v>
       </c>
       <c r="L141" s="7">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="33"/>
         <v>0</v>
       </c>
     </row>
@@ -55794,27 +57374,27 @@
         <v>16</v>
       </c>
       <c r="C142" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="D142" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="E142" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="F142" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="G142" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="H142" s="6">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="32"/>
         <v>28.1</v>
       </c>
       <c r="J142" s="6">
@@ -55822,7 +57402,7 @@
         <v>5.9</v>
       </c>
       <c r="L142" s="7">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="33"/>
         <v>0</v>
       </c>
     </row>
@@ -55845,7 +57425,15 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="88">
+  <mergeCells count="96">
+    <mergeCell ref="EO68:ET68"/>
+    <mergeCell ref="EO91:EV91"/>
+    <mergeCell ref="EA91:EH91"/>
+    <mergeCell ref="DP81:DW81"/>
+    <mergeCell ref="DP91:DW91"/>
+    <mergeCell ref="EA81:EH81"/>
+    <mergeCell ref="EA60:EH60"/>
+    <mergeCell ref="EA68:EH68"/>
     <mergeCell ref="DD40:DI40"/>
     <mergeCell ref="DD68:DK68"/>
     <mergeCell ref="DD60:DK60"/>

</xml_diff>